<commit_message>
update inviated speakers and program
</commit_message>
<xml_diff>
--- a/program/program.xlsx
+++ b/program/program.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24330" windowHeight="12675"/>
+    <workbookView windowWidth="24435" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>Program 11th Symposium on Ultrafast Surface Dynamics</t>
   </si>
@@ -46,84 +46,84 @@
     <t>Arrival Registration</t>
   </si>
   <si>
+    <t>Shiwei Wu</t>
+  </si>
+  <si>
+    <t>Xiaoyang Zhu</t>
+  </si>
+  <si>
+    <t>Christian Heide</t>
+  </si>
+  <si>
+    <t>Martin Wolf</t>
+  </si>
+  <si>
+    <t>Martin Weinelt</t>
+  </si>
+  <si>
+    <t>09:20</t>
+  </si>
+  <si>
+    <t>09:40</t>
+  </si>
+  <si>
+    <t>Martin Aeschlimann</t>
+  </si>
+  <si>
+    <t>Uwe Bovensiepen</t>
+  </si>
+  <si>
+    <t>Walter Pfeiffer</t>
+  </si>
+  <si>
+    <t>Shijing Tan</t>
+  </si>
+  <si>
+    <t>Ryuichi Arafune</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>Andreas Gebauer</t>
+  </si>
+  <si>
+    <t>10:20</t>
+  </si>
+  <si>
+    <t>Coffee Break</t>
+  </si>
+  <si>
+    <t>10:40</t>
+  </si>
+  <si>
+    <t>Robin Huang</t>
+  </si>
+  <si>
+    <t>Michael Bauer</t>
+  </si>
+  <si>
+    <t>Sheng Meng</t>
+  </si>
+  <si>
+    <t>Fengqiu Wang</t>
+  </si>
+  <si>
+    <t>Zhensheng Tao</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:20</t>
+  </si>
+  <si>
+    <t>Markus B. Raschke</t>
+  </si>
+  <si>
     <t>Javier García de Abajo</t>
   </si>
   <si>
-    <t>Xiaoyang Zhu</t>
-  </si>
-  <si>
-    <t>Christian Heide</t>
-  </si>
-  <si>
-    <t>Martin Wolf</t>
-  </si>
-  <si>
-    <t>Martin Weinelt</t>
-  </si>
-  <si>
-    <t>09:20</t>
-  </si>
-  <si>
-    <t>09:40</t>
-  </si>
-  <si>
-    <t>Martin Aeschlimann</t>
-  </si>
-  <si>
-    <t>Uwe Bovensiepen</t>
-  </si>
-  <si>
-    <t>Walter Pfeiffer</t>
-  </si>
-  <si>
-    <t>Shijing Tan</t>
-  </si>
-  <si>
-    <t>Ryuichi Arafune</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>Andreas Gebauer</t>
-  </si>
-  <si>
-    <t>10:20</t>
-  </si>
-  <si>
-    <t>Coffee Break</t>
-  </si>
-  <si>
-    <t>10:40</t>
-  </si>
-  <si>
-    <t>Robin Huang</t>
-  </si>
-  <si>
-    <t>Michael Bauer</t>
-  </si>
-  <si>
-    <t>Sheng Meng</t>
-  </si>
-  <si>
-    <t>Fengqiu Wang</t>
-  </si>
-  <si>
-    <t>Zhensheng Tao</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>11:20</t>
-  </si>
-  <si>
-    <t>Markus B. Raschke</t>
-  </si>
-  <si>
-    <t>Shiwei Wu</t>
-  </si>
-  <si>
     <t>Jin Zhao</t>
   </si>
   <si>
@@ -160,46 +160,49 @@
     <t>Oliver B. Wright</t>
   </si>
   <si>
+    <t>Kazuki Sumida</t>
+  </si>
+  <si>
+    <t>Lisa Grad</t>
+  </si>
+  <si>
+    <t>Timm Rohwer</t>
+  </si>
+  <si>
+    <t>Helmut Zacharias</t>
+  </si>
+  <si>
+    <t>Cheng-Tien Chiang</t>
+  </si>
+  <si>
     <t>Kaihui Liu</t>
   </si>
   <si>
-    <t>Lisa Grad</t>
-  </si>
-  <si>
-    <t>Timm Rohwer</t>
-  </si>
-  <si>
-    <t>Helmut Zacharias</t>
-  </si>
-  <si>
-    <t>Hadas Soifer</t>
-  </si>
-  <si>
-    <t>Cheng-Tien Chiang</t>
-  </si>
-  <si>
     <t>Kiyoshi Miyata</t>
   </si>
   <si>
+    <t>Sebastian F. Maehrlein</t>
+  </si>
+  <si>
+    <t>Henry Kapteyn</t>
+  </si>
+  <si>
     <t>Haiming Zhu</t>
   </si>
   <si>
-    <t>Sebastian F. Maehrlein</t>
-  </si>
-  <si>
-    <t>Henry Kapteyn</t>
-  </si>
-  <si>
     <t>Kunie Ishioka</t>
   </si>
   <si>
     <t>Dinner</t>
   </si>
   <si>
+    <t>Daniel Niesner</t>
+  </si>
+  <si>
     <t>Nan Pan</t>
   </si>
   <si>
-    <t>Daniel Niesner</t>
+    <t>Ti Wang</t>
   </si>
   <si>
     <t>Conference Dinner</t>
@@ -229,7 +232,7 @@
     <t>Poster Award</t>
   </si>
   <si>
-    <t>Invited Speaker</t>
+    <t xml:space="preserve">Invited Speaker </t>
   </si>
   <si>
     <t>Contributed Speaker</t>
@@ -240,9 +243,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -278,6 +281,142 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -285,142 +424,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -467,13 +470,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,13 +572,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,13 +608,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,133 +626,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,11 +795,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -818,6 +851,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -825,28 +869,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -865,181 +892,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1064,9 +1067,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1082,6 +1082,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1097,9 +1109,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,25 +1121,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1151,28 +1151,19 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1258,7 +1249,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1515,11 +1506,11 @@
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7142857142857" style="2" customWidth="1"/>
     <col min="2" max="7" width="20.7142857142857" style="3" customWidth="1"/>
@@ -1536,7 +1527,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="22"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" s="2" customFormat="1" ht="22" customHeight="1" spans="1:8">
       <c r="A2" s="6" t="s">
@@ -1560,28 +1551,28 @@
       <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" ht="16" customHeight="1" spans="1:7">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1590,30 +1581,30 @@
         <v>15</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:7">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1622,32 +1613,32 @@
         <v>22</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" ht="16" customHeight="1" spans="1:7">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1656,19 +1647,19 @@
         <v>26</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1677,131 +1668,131 @@
         <v>32</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" ht="16" customHeight="1" spans="1:7">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1" spans="1:7">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>0.486111111111111</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="27" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" ht="16" customHeight="1" spans="1:7">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>0.5</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="16" t="s">
         <v>39</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="29"/>
     </row>
     <row r="13" ht="16" customHeight="1" spans="1:7">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>0.513888888888889</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="28"/>
       <c r="G13" s="29"/>
     </row>
     <row r="14" ht="16" customHeight="1" spans="1:7">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>0.527777777777778</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="27"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="28"/>
       <c r="G14" s="29"/>
     </row>
     <row r="15" ht="16" customHeight="1" spans="1:7">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>0.541666666666667</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="27"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
     </row>
     <row r="16" ht="16" customHeight="1" spans="1:7">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>0.555555555555556</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
     </row>
     <row r="17" ht="16" customHeight="1" spans="1:7">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>0.569444444444444</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="27"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="28"/>
       <c r="G17" s="29"/>
     </row>
     <row r="18" ht="16" customHeight="1" spans="1:7">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>0.583333333333333</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="30" t="s">
         <v>43</v>
       </c>
@@ -1809,316 +1800,318 @@
       <c r="G18" s="29"/>
     </row>
     <row r="19" ht="16" customHeight="1" spans="1:7">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>0.597222222222222</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="21"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="29"/>
     </row>
     <row r="20" ht="16" customHeight="1" spans="1:7">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>0.611111111111111</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="9" t="s">
+      <c r="E20" s="31"/>
+      <c r="F20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="33"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" ht="16" customHeight="1" spans="1:7">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>0.625</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="33"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" ht="16" customHeight="1" spans="1:7">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>0.638888888888889</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="12" t="s">
+      <c r="E22" s="31"/>
+      <c r="F22" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" ht="16" customHeight="1" spans="1:7">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>0.652777777777778</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="12" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" ht="16" customHeight="1" spans="1:12">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>0.666666666666667</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="31"/>
+      <c r="F24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+    </row>
+    <row r="25" ht="16" customHeight="1" spans="1:7">
+      <c r="A25" s="10">
+        <v>0.680555555555556</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="33"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="45"/>
-    </row>
-    <row r="25" ht="16" customHeight="1" spans="1:7">
-      <c r="A25" s="11">
-        <v>0.680555555555556</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="12" t="s">
+      <c r="E25" s="33"/>
+      <c r="F25" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" ht="16" customHeight="1" spans="1:7">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>0.694444444444444</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="12" t="s">
+      <c r="G26" s="32"/>
+    </row>
+    <row r="27" ht="16" customHeight="1" spans="1:7">
+      <c r="A27" s="10">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" ht="16" customHeight="1" spans="1:7">
-      <c r="A27" s="11">
-        <v>0.708333333333333</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="12" t="s">
+      <c r="D27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="12" t="s">
+      <c r="E27" s="33"/>
+      <c r="F27" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G27" s="33"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" ht="16" customHeight="1" spans="1:7">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>0.722222222222222</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="14"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="12" t="s">
+      <c r="G28" s="32"/>
+    </row>
+    <row r="29" ht="16" customHeight="1" spans="1:7">
+      <c r="A29" s="10">
+        <v>0.736111111111111</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="33"/>
-    </row>
-    <row r="29" ht="16" customHeight="1" spans="1:7">
-      <c r="A29" s="11">
-        <v>0.736111111111111</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="15" t="s">
+      <c r="E29" s="33"/>
+      <c r="F29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="32"/>
+    </row>
+    <row r="30" ht="16" customHeight="1" spans="1:7">
+      <c r="A30" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="33"/>
-    </row>
-    <row r="30" ht="16" customHeight="1" spans="1:7">
-      <c r="A30" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="36" t="s">
+      <c r="E30" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="F30" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" ht="16" customHeight="1" spans="1:7">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>0.763888888888889</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="33"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" ht="16" customHeight="1" spans="1:7">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>0.777777777777778</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="33"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" ht="16" customHeight="1" spans="1:7">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>0.791666666666667</v>
       </c>
       <c r="B33" s="6"/>
-      <c r="C33" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="33"/>
+      <c r="C33" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" ht="16" customHeight="1" spans="1:7">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>0.805555555555556</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="33"/>
+      <c r="B34" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" ht="16" customHeight="1" spans="1:7">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>0.819444444444444</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="33"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" ht="16" customHeight="1" spans="1:7">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>0.833333333333333</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="33"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" ht="16" customHeight="1" spans="1:7">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>0.847222222222222</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G37" s="33"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" ht="16" customHeight="1" spans="1:7">
-      <c r="A38" s="11">
+      <c r="A38" s="10">
         <v>0.861111111111111</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="33"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" ht="16" customHeight="1" spans="1:7">
-      <c r="A39" s="20">
+      <c r="A39" s="22">
         <v>0.875</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="39"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="37"/>
     </row>
     <row r="41" spans="6:7">
-      <c r="F41" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="41" t="s">
+      <c r="F41" s="38" t="s">
         <v>72</v>
       </c>
+      <c r="G41" s="39" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="6:7">
-      <c r="F42" s="42"/>
-      <c r="G42" s="43"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="44">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B3:B33"/>
     <mergeCell ref="B35:B36"/>
@@ -2139,8 +2132,9 @@
     <mergeCell ref="D13:D19"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D30:D32"/>
     <mergeCell ref="D33:D38"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E8:E9"/>

</xml_diff>